<commit_message>
Added engineering floor data
</commit_message>
<xml_diff>
--- a/my-vue-app/UNO seats per room.xlsx
+++ b/my-vue-app/UNO seats per room.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\school\capstone\Team5-PKI_Scheduler\python-db\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\school\capstone\Team5-PKI_Scheduler\my-vue-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBF2FED-D37B-4AAB-A839-093AABCB6867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCBB744-474D-4D3F-8B13-CEB0131A0964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
+    <workbookView xWindow="32400" yWindow="0" windowWidth="6105" windowHeight="20985" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751ECBA2-A47A-40DA-932A-721630D732F7}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G33:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,6 +746,38 @@
         <v>8</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>117</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>127</v>
+      </c>
+      <c r="B40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>130</v>
+      </c>
+      <c r="B41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>248</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Crosslisted csv includes new data for maximum enrollment header. Reformated uno seats per room csv for excel vlookup formula to function
</commit_message>
<xml_diff>
--- a/my-vue-app/UNO seats per room.xlsx
+++ b/my-vue-app/UNO seats per room.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\school\capstone\Team5-PKI_Scheduler\my-vue-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCBB744-474D-4D3F-8B13-CEB0131A0964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A424697A-2F38-4202-A87C-5585CA726DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="0" windowWidth="6105" windowHeight="20985" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
+    <workbookView minimized="1" xWindow="-16050" yWindow="2070" windowWidth="16125" windowHeight="15345" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Room</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>154F</t>
+  </si>
+  <si>
+    <t>Room Helper</t>
   </si>
 </sst>
 </file>
@@ -434,347 +437,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751ECBA2-A47A-40DA-932A-721630D732F7}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G34" sqref="G33:G34"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>108</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
+        <f>TEXT(A2, 0)</f>
+        <v>108</v>
+      </c>
+      <c r="C2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>150</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B42" si="0">TEXT(A3, 0)</f>
+        <v>150</v>
+      </c>
+      <c r="C3">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>153</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+      <c r="C4">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>155</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="C5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>157</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+      <c r="C6">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>160</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C7">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>161</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="C8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>164</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="C9">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>250</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C10">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>252</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="C11">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>256</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="C12">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>259</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+      <c r="C13">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>260</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="C14">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>261</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+      <c r="C15">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>263</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>263</v>
+      </c>
+      <c r="C16">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>269</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>269</v>
+      </c>
+      <c r="C17">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>270</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="C18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>274</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+      <c r="C19">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>276</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+      <c r="C20">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>278</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>278</v>
+      </c>
+      <c r="C21">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>279</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>279</v>
+      </c>
+      <c r="C22">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>350</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="C23">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>361</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+      <c r="C24">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>391A</v>
+      </c>
+      <c r="C25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>145</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="C26">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>149</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="C27">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>151</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="C28">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>158</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="C29">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>249</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+      <c r="C30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>352</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="C31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>368</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+      <c r="C32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>154A</v>
+      </c>
+      <c r="C33">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>154B</v>
+      </c>
+      <c r="C34">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>154C</v>
+      </c>
+      <c r="C35">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>154D</v>
+      </c>
+      <c r="C36">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>154E</v>
+      </c>
+      <c r="C37">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>154F</v>
+      </c>
+      <c r="C38">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>117</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C39">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>127</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="C40">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>130</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C41">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>TEXT(248, 0)</f>
         <v>248</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="C42">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reformatted csv file for vlookup function and updated file with additional room data per sponsor
</commit_message>
<xml_diff>
--- a/my-vue-app/UNO seats per room.xlsx
+++ b/my-vue-app/UNO seats per room.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\school\capstone\Team5-PKI_Scheduler\python-db\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\school\capstone\Team5-PKI_Scheduler\my-vue-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBF2FED-D37B-4AAB-A839-093AABCB6867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A424697A-2F38-4202-A87C-5585CA726DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
+    <workbookView minimized="1" xWindow="-16050" yWindow="2070" windowWidth="16125" windowHeight="15345" xr2:uid="{A108EA3A-3851-48F9-AAE7-10E16BE1D56E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Room</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>154F</t>
+  </si>
+  <si>
+    <t>Room Helper</t>
   </si>
 </sst>
 </file>
@@ -434,316 +437,516 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751ECBA2-A47A-40DA-932A-721630D732F7}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>108</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
+        <f>TEXT(A2, 0)</f>
+        <v>108</v>
+      </c>
+      <c r="C2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>150</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B42" si="0">TEXT(A3, 0)</f>
+        <v>150</v>
+      </c>
+      <c r="C3">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>153</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+      <c r="C4">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>155</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="C5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>157</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+      <c r="C6">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>160</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C7">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>161</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="C8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>164</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="C9">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>250</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C10">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>252</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="C11">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>256</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="C12">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>259</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+      <c r="C13">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>260</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="C14">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>261</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>261</v>
+      </c>
+      <c r="C15">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>263</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>263</v>
+      </c>
+      <c r="C16">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>269</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>269</v>
+      </c>
+      <c r="C17">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>270</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="C18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>274</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+      <c r="C19">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>276</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+      <c r="C20">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>278</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>278</v>
+      </c>
+      <c r="C21">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>279</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>279</v>
+      </c>
+      <c r="C22">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>350</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="C23">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>361</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+      <c r="C24">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>391A</v>
+      </c>
+      <c r="C25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>145</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="C26">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>149</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="C27">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>151</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="C28">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>158</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="C29">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>249</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+      <c r="C30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>352</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>352</v>
+      </c>
+      <c r="C31">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>368</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>368</v>
+      </c>
+      <c r="C32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>154A</v>
+      </c>
+      <c r="C33">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>154B</v>
+      </c>
+      <c r="C34">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>154C</v>
+      </c>
+      <c r="C35">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>154D</v>
+      </c>
+      <c r="C36">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>154E</v>
+      </c>
+      <c r="C37">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>154F</v>
+      </c>
+      <c r="C38">
         <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>117</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="C39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>127</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="C40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>130</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>TEXT(248, 0)</f>
+        <v>248</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>